<commit_message>
bug fixes + Share
</commit_message>
<xml_diff>
--- a/ZZ_project features checklist.xlsx
+++ b/ZZ_project features checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="284" documentId="13_ncr:1_{B96D5725-443F-4501-A726-D0FF87981D2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A710B44D-ABE6-4304-8C86-E203C3E95A7D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="-15420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A57" activeCellId="1" sqref="A60 A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>